<commit_message>
add check user address
</commit_message>
<xml_diff>
--- a/storage/template/school-importing-template.xlsx
+++ b/storage/template/school-importing-template.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22307"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_81E8B0FE38E28F01AA3564782D074E64CFFAB842" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1AC527C8-3A04-4970-B8B6-23DB056C1B2C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Imported Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -25,11 +37,14 @@
             <rFont val="Helvetica Neue"/>
           </rPr>
           <t>Imported Author:
-** ไม่ต้องใส่คำว่า โรงเรียนนำหน้า</t>
+Optional: ใส่หรือไม่ใส่ก็ได้
+Value: 1 สถานะใช้งาน, 0 ระงับการใช้งาน
+Default: 1
+	-Nuttasak Tawan</t>
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <r>
       <rPr>
@@ -111,10 +126,13 @@
     <t>สังกัดของโรงเรียน</t>
   </si>
   <si>
+    <t>สถานะ</t>
+  </si>
+  <si>
     <t>หมายเหตุ</t>
   </si>
   <si>
-    <t>สามเสนวิทยาลัย</t>
+    <t>สกลราชวิทยานุกูล</t>
   </si>
   <si>
     <t>11/11</t>
@@ -135,29 +153,16 @@
     <t>กรุงเทพมหานคร</t>
   </si>
   <si>
-    <t>สำนักงานคณะกรรมการการศึกษาขั้นพื้นฐาน</t>
+    <t>สพฐ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
@@ -191,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -243,92 +248,106 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ff38761d"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FF38761D"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -460,7 +479,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -536,7 +555,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -555,7 +574,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -585,7 +604,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -611,7 +630,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -637,7 +656,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -663,7 +682,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -689,7 +708,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -715,7 +734,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -741,7 +760,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -767,7 +786,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -793,7 +812,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -806,9 +825,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -823,7 +848,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="38000"/>
             </a:srgbClr>
@@ -831,7 +856,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -850,7 +875,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -876,7 +901,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -902,7 +927,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -928,7 +953,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -954,7 +979,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -980,7 +1005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1006,7 +1031,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1032,7 +1057,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1058,7 +1083,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1084,7 +1109,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1097,9 +1122,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1113,7 +1144,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1132,7 +1163,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1162,7 +1193,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1188,7 +1219,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1214,7 +1245,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1240,7 +1271,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1266,7 +1297,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1292,7 +1323,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1318,7 +1349,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1344,7 +1375,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1370,7 +1401,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,216 +1414,121 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:IV2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.6719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.3516" style="1" customWidth="1"/>
-    <col min="3" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1719" style="1" customWidth="1"/>
-    <col min="6" max="9" width="14.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.3516" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" style="1" customWidth="1"/>
-    <col min="12" max="256" width="14.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="1" customWidth="1"/>
+    <col min="3" max="9" width="14.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="1" customWidth="1"/>
+    <col min="11" max="256" width="14.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.3" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:12" ht="16.350000000000001" customHeight="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="3">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="3">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="3">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="3">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="4">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="5">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s" s="6">
+    <row r="2" spans="1:12" ht="13.7" customHeight="1">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="7">
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6">
         <v>1</v>
       </c>
-      <c r="D2" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s" s="5">
+      <c r="D2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s" s="5">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s" s="5">
+      <c r="F2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s" s="5">
+      <c r="G2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8">
-        <v>10400</v>
-      </c>
-      <c r="J2" t="s" s="5">
+      <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
+      <c r="I2" s="6">
+        <v>102800</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>